<commit_message>
Add wikidata-query Code tweaks
</commit_message>
<xml_diff>
--- a/app/Resources/data/gnd2tgn.xlsx
+++ b/app/Resources/data/gnd2tgn.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>place</t>
   </si>
@@ -34,6 +34,105 @@
   </si>
   <si>
     <t>http://d-nb.info/gnd/4546481-9</t>
+  </si>
+  <si>
+    <t>Neuhaus im Solling</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/2020253-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1040455</t>
+  </si>
+  <si>
+    <t>Jerusalem</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4028586-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7001371</t>
+  </si>
+  <si>
+    <t>Lübeck</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4036483-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012327</t>
+  </si>
+  <si>
+    <t>Celle</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4009657-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005317</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4068038-1</t>
+  </si>
+  <si>
+    <t>Zürich</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007302</t>
+  </si>
+  <si>
+    <t>Herne</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4024544-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1039566</t>
+  </si>
+  <si>
+    <t>Leipzig</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4035206-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012329</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7018159</t>
+  </si>
+  <si>
+    <t>Venice</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4062501-1:</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004446</t>
+  </si>
+  <si>
+    <t>Köln</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4031483-2</t>
+  </si>
+  <si>
+    <t>Kopenhagen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4032399-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7003474</t>
+  </si>
+  <si>
+    <t>Bern</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4005762-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007557</t>
   </si>
 </sst>
 </file>
@@ -368,14 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
   <cols>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="5" max="5" width="28.125" customWidth="1"/>
     <col min="6" max="6" width="37.75" customWidth="1"/>
@@ -404,6 +505,127 @@
         <v>4</v>
       </c>
       <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add new Place.type Add missing translation
</commit_message>
<xml_diff>
--- a/app/Resources/data/gnd2tgn.xlsx
+++ b/app/Resources/data/gnd2tgn.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="129">
   <si>
     <t>place</t>
   </si>
@@ -133,6 +133,276 @@
   </si>
   <si>
     <t>http://vocab.getty.edu/tgn/7007557</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1048994</t>
+  </si>
+  <si>
+    <t>Czempiń</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/10022243-2</t>
+  </si>
+  <si>
+    <t>Krotoszyn</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049186</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/301975-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005985</t>
+  </si>
+  <si>
+    <t>Aalen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4000015-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7006952</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4001783-7</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Baden-Baden</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005172</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4004169-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007269</t>
+  </si>
+  <si>
+    <t>Basel</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4004617-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004326</t>
+  </si>
+  <si>
+    <t>Bayreuth</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4005056-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1036449</t>
+  </si>
+  <si>
+    <t>Bernburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4005774-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005090</t>
+  </si>
+  <si>
+    <t>Bonn</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4007666-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7003283</t>
+  </si>
+  <si>
+    <t>Braunau am Inn</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4008037-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005286</t>
+  </si>
+  <si>
+    <t>Bremen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4008135-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007601</t>
+  </si>
+  <si>
+    <t>Breslau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4008216-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007660</t>
+  </si>
+  <si>
+    <t>Danzig</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4011039-4</t>
+  </si>
+  <si>
+    <t>Darmstadt</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004428</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4011077-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007342</t>
+  </si>
+  <si>
+    <t>Davos</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4011220-2</t>
+  </si>
+  <si>
+    <t>Dessau</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012804</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4011536-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004455</t>
+  </si>
+  <si>
+    <t>Dresden</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4012995-0</t>
+  </si>
+  <si>
+    <t>Düsseldorf</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004443</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4013255-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012432</t>
+  </si>
+  <si>
+    <t>Eckernförde</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4013498-2</t>
+  </si>
+  <si>
+    <t>Eisenach</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005969</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4014013-1</t>
+  </si>
+  <si>
+    <t>Erlangen</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004332</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4015299-6</t>
+  </si>
+  <si>
+    <t>Frankfurt am Main</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4018118-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005293</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004423</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4018272-1</t>
+  </si>
+  <si>
+    <t>Freiburg im Breisgau</t>
+  </si>
+  <si>
+    <t>Genf</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007279</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4020137-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004429</t>
+  </si>
+  <si>
+    <t>Gießen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4020989-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012813</t>
+  </si>
+  <si>
+    <t>Görlitz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4021441-2</t>
+  </si>
+  <si>
+    <t>Göttingen</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005246</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4021477-1</t>
+  </si>
+  <si>
+    <t>Hechingen</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1039493</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4023927-5</t>
+  </si>
+  <si>
+    <t>Kamen</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1039810</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4029404-3</t>
+  </si>
+  <si>
+    <t>Chemnitz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4029702-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005951</t>
   </si>
 </sst>
 </file>
@@ -467,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
@@ -625,6 +895,347 @@
       </c>
       <c r="C13" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" t="s">
+        <v>71</v>
+      </c>
+      <c r="C24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B25" t="s">
+        <v>74</v>
+      </c>
+      <c r="C25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>76</v>
+      </c>
+      <c r="B26" t="s">
+        <v>77</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>78</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C32" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>107</v>
+      </c>
+      <c r="B36" t="s">
+        <v>106</v>
+      </c>
+      <c r="C36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>112</v>
+      </c>
+      <c r="B38" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>115</v>
+      </c>
+      <c r="B39" t="s">
+        <v>116</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>117</v>
+      </c>
+      <c r="B40" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>120</v>
+      </c>
+      <c r="B41" t="s">
+        <v>122</v>
+      </c>
+      <c r="C41" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>123</v>
+      </c>
+      <c r="B43" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>126</v>
+      </c>
+      <c r="B44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add boundaries (ISO 3166-2)
</commit_message>
<xml_diff>
--- a/app/Resources/data/gnd2tgn.xlsx
+++ b/app/Resources/data/gnd2tgn.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="503">
   <si>
     <t>place</t>
   </si>
@@ -571,6 +571,960 @@
   </si>
   <si>
     <t>http://d-nb.info/gnd/4059353-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1004170</t>
+  </si>
+  <si>
+    <t>Wien-Brigittenau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4108149-3</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7003468</t>
+  </si>
+  <si>
+    <t>Amt Frederiksborg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4566680-5</t>
+  </si>
+  <si>
+    <t>Landsberg (Warthe)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4034340-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007720</t>
+  </si>
+  <si>
+    <t>Sprendlingen (Dreieich)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4105504-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7097684</t>
+  </si>
+  <si>
+    <t>Recklinghausen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4048864-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005083</t>
+  </si>
+  <si>
+    <t>Rehau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4049080-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1040847</t>
+  </si>
+  <si>
+    <t>Rosenheim</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4050554-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004690</t>
+  </si>
+  <si>
+    <t>Lüneburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4036512-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004436</t>
+  </si>
+  <si>
+    <t>Ried im Innkreis</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4104043-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7003281</t>
+  </si>
+  <si>
+    <t>Schlawe in Pommern</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4252282-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049438</t>
+  </si>
+  <si>
+    <t>Neu-Isenburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4041799-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012521</t>
+  </si>
+  <si>
+    <t>Doorn</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4091147-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7006911</t>
+  </si>
+  <si>
+    <t>Spandau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4105431-3</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1005645</t>
+  </si>
+  <si>
+    <t>Alsenz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4085003-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1038159</t>
+  </si>
+  <si>
+    <t>Rheydt</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4049838-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004976</t>
+  </si>
+  <si>
+    <t>Mannheim</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4037372-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7005179</t>
+  </si>
+  <si>
+    <t>Wittlich</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4066668-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1041861</t>
+  </si>
+  <si>
+    <t>Wolfsburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4066874-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012783</t>
+  </si>
+  <si>
+    <t>Burgdorf (Region Hannover)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4009112-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1038693</t>
+  </si>
+  <si>
+    <t>Laupheim</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4034744-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1040058</t>
+  </si>
+  <si>
+    <t>Auschwitz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4068979-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7013310</t>
+  </si>
+  <si>
+    <t>Reutlingen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4049657-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012674</t>
+  </si>
+  <si>
+    <t>Krakau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4073760-3</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007652</t>
+  </si>
+  <si>
+    <t>Zierenberg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4067754-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1041913</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012468</t>
+  </si>
+  <si>
+    <t>Garding</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4254826-3</t>
+  </si>
+  <si>
+    <t>Los Angeles, Calif.</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4036361-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7023900</t>
+  </si>
+  <si>
+    <t>Reichenberg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4103609-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7011694</t>
+  </si>
+  <si>
+    <t>Falkenstein-Ermsleben</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4335999-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1036667</t>
+  </si>
+  <si>
+    <t>Oettingen i. Bay.</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4116730-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012633</t>
+  </si>
+  <si>
+    <t>Laufen (Berchtesgadener Land)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4034720-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012566</t>
+  </si>
+  <si>
+    <t>Straubing</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4057970-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004413</t>
+  </si>
+  <si>
+    <t>Rammenau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4368618-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7109920</t>
+  </si>
+  <si>
+    <t>Carouge</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4395194-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007333</t>
+  </si>
+  <si>
+    <t>Rochester (Kent)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4404644-3</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7011707</t>
+  </si>
+  <si>
+    <t>Karlsbad</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4029705-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7011521</t>
+  </si>
+  <si>
+    <t>Deutz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4321358-3</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/4003264</t>
+  </si>
+  <si>
+    <t>Wernigerode</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4065649-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012889</t>
+  </si>
+  <si>
+    <t>Ermenonville</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4342057-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7009163</t>
+  </si>
+  <si>
+    <t>Kirkcaldy</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4030852-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7009919</t>
+  </si>
+  <si>
+    <t>Sos del Rey Católico</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4718776-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007613</t>
+  </si>
+  <si>
+    <t>Medina del Campo</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4394975-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7008033</t>
+  </si>
+  <si>
+    <t>Hyde Park, NY</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4220508-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7013733</t>
+  </si>
+  <si>
+    <t>Warm Springs, Ga.</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4438479-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/2024654</t>
+  </si>
+  <si>
+    <t>Pest (Stadt)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4137172-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7010546</t>
+  </si>
+  <si>
+    <t>Planegg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4103120-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1040744</t>
+  </si>
+  <si>
+    <t>Giverny</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4021113-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7009209</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7018662</t>
+  </si>
+  <si>
+    <t>Charlotte Amalie</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/16339843-4</t>
+  </si>
+  <si>
+    <t>Kamenz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4029407-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012829</t>
+  </si>
+  <si>
+    <t>Santa Eulalia del Rio</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/7514598-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1062487</t>
+  </si>
+  <si>
+    <t>Prerau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4466766-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1027451</t>
+  </si>
+  <si>
+    <t>Banyuls-sur-Mer</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4252712-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/4001198</t>
+  </si>
+  <si>
+    <t>Visp</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4108304-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007494</t>
+  </si>
+  <si>
+    <t>Bergen-Belsen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4129487-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7075381</t>
+  </si>
+  <si>
+    <t>Waldenburg (Schlesien)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4118961-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049581</t>
+  </si>
+  <si>
+    <t>Ludwigsstadt</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4111414-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012587</t>
+  </si>
+  <si>
+    <t>Ajaccio</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4212951-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7008351</t>
+  </si>
+  <si>
+    <t>Neukölln</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4102500-3</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1005180</t>
+  </si>
+  <si>
+    <t>Schönhausen (Elbe)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4296831-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1037660</t>
+  </si>
+  <si>
+    <t>Aumühle-Friedrichsruh</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4093323-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7182429</t>
+  </si>
+  <si>
+    <t>Gries (Bozen)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4536127-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/4004583</t>
+  </si>
+  <si>
+    <t>Neustrelitz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4101150-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1037377</t>
+  </si>
+  <si>
+    <t>Zamość</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4248619-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007840</t>
+  </si>
+  <si>
+    <t>Capri</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4009452-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1043863</t>
+  </si>
+  <si>
+    <t>Lemgo</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4035306-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012571</t>
+  </si>
+  <si>
+    <t>Wipperdorf</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4794279-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1038005</t>
+  </si>
+  <si>
+    <t>Allenstein</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4001252-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007583</t>
+  </si>
+  <si>
+    <t>Oranienburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4043700-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1037432</t>
+  </si>
+  <si>
+    <t>Szamocin</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4674417-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049514</t>
+  </si>
+  <si>
+    <t>Lissa</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4330219-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049207</t>
+  </si>
+  <si>
+    <t>Bocholt</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4007326-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1038566</t>
+  </si>
+  <si>
+    <t>Landsberg (Oberschlesien)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/118713-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049061</t>
+  </si>
+  <si>
+    <t>Weißenburg i. Bay.</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4065243-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7085374</t>
+  </si>
+  <si>
+    <t>Dolsk (Woiwodschaft Großpolen)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4559988-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049015</t>
+  </si>
+  <si>
+    <t>Reval</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4076684-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7006629</t>
+  </si>
+  <si>
+    <t>Pforzheim</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4045637-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012653</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1005565</t>
+  </si>
+  <si>
+    <t>Berlin-Schöneberg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4087340-7</t>
+  </si>
+  <si>
+    <t>Ludwigshafen am Rhein</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4036472-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012586</t>
+  </si>
+  <si>
+    <t>Mainz-Weisenau</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4100030-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7086133</t>
+  </si>
+  <si>
+    <t>Detmold</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4011555-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004442</t>
+  </si>
+  <si>
+    <t>Zabrze</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4089236-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1049628</t>
+  </si>
+  <si>
+    <t>Lemberg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4035304-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7003382</t>
+  </si>
+  <si>
+    <t>Mölln</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4039901-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1040184</t>
+  </si>
+  <si>
+    <t>Chicago, Ill.</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4009921-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7017994</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7013596</t>
+  </si>
+  <si>
+    <t>Budapest</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4008684-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7000457</t>
+  </si>
+  <si>
+    <t>Florenz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4017581-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7013625</t>
+  </si>
+  <si>
+    <t>Durham, NC</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4199417-6</t>
+  </si>
+  <si>
+    <t>Geesthacht</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4019635-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1039204</t>
+  </si>
+  <si>
+    <t>Sansepolcro</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4246244-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7000478</t>
+  </si>
+  <si>
+    <t>Argentan</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4246454-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7008654</t>
+  </si>
+  <si>
+    <t>Gif-sur-Yvette</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4350189-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7009204</t>
+  </si>
+  <si>
+    <t>Málaga</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4100040-7</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007942</t>
+  </si>
+  <si>
+    <t>Mougins</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4534855-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/4007565</t>
+  </si>
+  <si>
+    <t>Verona</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4063110-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7003262</t>
+  </si>
+  <si>
+    <t>Bingen am Rhein</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4006753-1</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012309</t>
+  </si>
+  <si>
+    <t>Kattowitz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4097725-0</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007685</t>
+  </si>
+  <si>
+    <t>Cincinnati, Ohio</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4085269-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7013604</t>
+  </si>
+  <si>
+    <t>Wurz (Püchersreuth)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4260157-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7078670</t>
+  </si>
+  <si>
+    <t>Warburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4064574-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012758</t>
+  </si>
+  <si>
+    <t>Stratford-upon-Avon</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4118849-4</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7010956</t>
+  </si>
+  <si>
+    <t>Kapstadt</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4029615-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7000811</t>
+  </si>
+  <si>
+    <t>Koblenz</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4031410-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004448</t>
+  </si>
+  <si>
+    <t>Augsburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4003614-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004324</t>
+  </si>
+  <si>
+    <t>Arnsberg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4003007-6</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7062247</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7012573</t>
+  </si>
+  <si>
+    <t>Leverkusen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4035513-5</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7004905</t>
+  </si>
+  <si>
+    <t>Essen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4015557-2</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1039548</t>
+  </si>
+  <si>
+    <t>Henstedt-Ulzburg</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4224404-3</t>
   </si>
 </sst>
 </file>
@@ -905,10 +1859,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:F169"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
@@ -1613,6 +2567,1172 @@
       </c>
       <c r="C63" t="s">
         <v>183</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>186</v>
+      </c>
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>191</v>
+      </c>
+      <c r="B66" t="s">
+        <v>192</v>
+      </c>
+      <c r="C66" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>194</v>
+      </c>
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>197</v>
+      </c>
+      <c r="B68" t="s">
+        <v>198</v>
+      </c>
+      <c r="C68" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>200</v>
+      </c>
+      <c r="B69" t="s">
+        <v>201</v>
+      </c>
+      <c r="C69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>203</v>
+      </c>
+      <c r="B70" t="s">
+        <v>204</v>
+      </c>
+      <c r="C70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71" t="s">
+        <v>207</v>
+      </c>
+      <c r="C71" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>209</v>
+      </c>
+      <c r="B72" t="s">
+        <v>210</v>
+      </c>
+      <c r="C72" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>212</v>
+      </c>
+      <c r="B73" t="s">
+        <v>213</v>
+      </c>
+      <c r="C73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>215</v>
+      </c>
+      <c r="B74" t="s">
+        <v>216</v>
+      </c>
+      <c r="C74" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>218</v>
+      </c>
+      <c r="B75" t="s">
+        <v>219</v>
+      </c>
+      <c r="C75" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>221</v>
+      </c>
+      <c r="B76" t="s">
+        <v>222</v>
+      </c>
+      <c r="C76" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>224</v>
+      </c>
+      <c r="B77" t="s">
+        <v>225</v>
+      </c>
+      <c r="C77" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>227</v>
+      </c>
+      <c r="B78" t="s">
+        <v>228</v>
+      </c>
+      <c r="C78" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>230</v>
+      </c>
+      <c r="B79" t="s">
+        <v>231</v>
+      </c>
+      <c r="C79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>233</v>
+      </c>
+      <c r="B80" t="s">
+        <v>234</v>
+      </c>
+      <c r="C80" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>236</v>
+      </c>
+      <c r="B81" t="s">
+        <v>237</v>
+      </c>
+      <c r="C81" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>239</v>
+      </c>
+      <c r="B82" t="s">
+        <v>240</v>
+      </c>
+      <c r="C82" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>242</v>
+      </c>
+      <c r="B83" t="s">
+        <v>243</v>
+      </c>
+      <c r="C83" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>245</v>
+      </c>
+      <c r="B84" t="s">
+        <v>246</v>
+      </c>
+      <c r="C84" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>248</v>
+      </c>
+      <c r="B85" t="s">
+        <v>249</v>
+      </c>
+      <c r="C85" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>251</v>
+      </c>
+      <c r="B86" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>254</v>
+      </c>
+      <c r="B87" t="s">
+        <v>255</v>
+      </c>
+      <c r="C87" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>258</v>
+      </c>
+      <c r="B88" t="s">
+        <v>259</v>
+      </c>
+      <c r="C88" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>260</v>
+      </c>
+      <c r="B89" t="s">
+        <v>261</v>
+      </c>
+      <c r="C89" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>263</v>
+      </c>
+      <c r="B90" t="s">
+        <v>264</v>
+      </c>
+      <c r="C90" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>266</v>
+      </c>
+      <c r="B91" t="s">
+        <v>267</v>
+      </c>
+      <c r="C91" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>269</v>
+      </c>
+      <c r="B92" t="s">
+        <v>270</v>
+      </c>
+      <c r="C92" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>272</v>
+      </c>
+      <c r="B93" t="s">
+        <v>273</v>
+      </c>
+      <c r="C93" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>275</v>
+      </c>
+      <c r="B94" t="s">
+        <v>276</v>
+      </c>
+      <c r="C94" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>278</v>
+      </c>
+      <c r="B95" t="s">
+        <v>279</v>
+      </c>
+      <c r="C95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>281</v>
+      </c>
+      <c r="B96" t="s">
+        <v>282</v>
+      </c>
+      <c r="C96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" t="s">
+        <v>285</v>
+      </c>
+      <c r="C97" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>287</v>
+      </c>
+      <c r="B98" t="s">
+        <v>288</v>
+      </c>
+      <c r="C98" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>290</v>
+      </c>
+      <c r="B99" t="s">
+        <v>291</v>
+      </c>
+      <c r="C99" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>293</v>
+      </c>
+      <c r="B100" t="s">
+        <v>294</v>
+      </c>
+      <c r="C100" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>296</v>
+      </c>
+      <c r="B101" t="s">
+        <v>297</v>
+      </c>
+      <c r="C101" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>299</v>
+      </c>
+      <c r="B102" t="s">
+        <v>300</v>
+      </c>
+      <c r="C102" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>302</v>
+      </c>
+      <c r="B103" t="s">
+        <v>303</v>
+      </c>
+      <c r="C103" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>305</v>
+      </c>
+      <c r="B104" t="s">
+        <v>306</v>
+      </c>
+      <c r="C104" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>308</v>
+      </c>
+      <c r="B105" t="s">
+        <v>309</v>
+      </c>
+      <c r="C105" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>311</v>
+      </c>
+      <c r="B106" t="s">
+        <v>312</v>
+      </c>
+      <c r="C106" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>314</v>
+      </c>
+      <c r="B107" t="s">
+        <v>315</v>
+      </c>
+      <c r="C107" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>317</v>
+      </c>
+      <c r="B108" t="s">
+        <v>318</v>
+      </c>
+      <c r="C108" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>320</v>
+      </c>
+      <c r="B109" t="s">
+        <v>321</v>
+      </c>
+      <c r="C109" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>324</v>
+      </c>
+      <c r="B110" t="s">
+        <v>325</v>
+      </c>
+      <c r="C110" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>326</v>
+      </c>
+      <c r="B111" t="s">
+        <v>327</v>
+      </c>
+      <c r="C111" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>329</v>
+      </c>
+      <c r="B112" t="s">
+        <v>330</v>
+      </c>
+      <c r="C112" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>332</v>
+      </c>
+      <c r="B113" t="s">
+        <v>333</v>
+      </c>
+      <c r="C113" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>335</v>
+      </c>
+      <c r="B114" t="s">
+        <v>336</v>
+      </c>
+      <c r="C114" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>338</v>
+      </c>
+      <c r="B115" t="s">
+        <v>339</v>
+      </c>
+      <c r="C115" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>341</v>
+      </c>
+      <c r="B116" t="s">
+        <v>342</v>
+      </c>
+      <c r="C116" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>344</v>
+      </c>
+      <c r="B117" t="s">
+        <v>345</v>
+      </c>
+      <c r="C117" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>347</v>
+      </c>
+      <c r="B118" t="s">
+        <v>348</v>
+      </c>
+      <c r="C118" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>350</v>
+      </c>
+      <c r="B119" t="s">
+        <v>351</v>
+      </c>
+      <c r="C119" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>353</v>
+      </c>
+      <c r="B120" t="s">
+        <v>354</v>
+      </c>
+      <c r="C120" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>356</v>
+      </c>
+      <c r="B121" t="s">
+        <v>357</v>
+      </c>
+      <c r="C121" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>359</v>
+      </c>
+      <c r="B122" t="s">
+        <v>360</v>
+      </c>
+      <c r="C122" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>362</v>
+      </c>
+      <c r="B123" t="s">
+        <v>363</v>
+      </c>
+      <c r="C123" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>365</v>
+      </c>
+      <c r="B124" t="s">
+        <v>366</v>
+      </c>
+      <c r="C124" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>368</v>
+      </c>
+      <c r="B125" t="s">
+        <v>369</v>
+      </c>
+      <c r="C125" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>371</v>
+      </c>
+      <c r="B126" t="s">
+        <v>372</v>
+      </c>
+      <c r="C126" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" t="s">
+        <v>374</v>
+      </c>
+      <c r="B127" t="s">
+        <v>375</v>
+      </c>
+      <c r="C127" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" t="s">
+        <v>377</v>
+      </c>
+      <c r="B128" t="s">
+        <v>378</v>
+      </c>
+      <c r="C128" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3">
+      <c r="A129" t="s">
+        <v>380</v>
+      </c>
+      <c r="B129" t="s">
+        <v>381</v>
+      </c>
+      <c r="C129" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3">
+      <c r="A130" t="s">
+        <v>383</v>
+      </c>
+      <c r="B130" t="s">
+        <v>384</v>
+      </c>
+      <c r="C130" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3">
+      <c r="A131" t="s">
+        <v>386</v>
+      </c>
+      <c r="B131" t="s">
+        <v>387</v>
+      </c>
+      <c r="C131" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3">
+      <c r="A132" t="s">
+        <v>389</v>
+      </c>
+      <c r="B132" t="s">
+        <v>390</v>
+      </c>
+      <c r="C132" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3">
+      <c r="A133" t="s">
+        <v>392</v>
+      </c>
+      <c r="B133" t="s">
+        <v>393</v>
+      </c>
+      <c r="C133" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3">
+      <c r="A134" t="s">
+        <v>395</v>
+      </c>
+      <c r="B134" t="s">
+        <v>396</v>
+      </c>
+      <c r="C134" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3">
+      <c r="A135" t="s">
+        <v>398</v>
+      </c>
+      <c r="B135" t="s">
+        <v>399</v>
+      </c>
+      <c r="C135" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3">
+      <c r="A136" t="s">
+        <v>401</v>
+      </c>
+      <c r="B136" t="s">
+        <v>402</v>
+      </c>
+      <c r="C136" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3">
+      <c r="A137" t="s">
+        <v>404</v>
+      </c>
+      <c r="B137" t="s">
+        <v>405</v>
+      </c>
+      <c r="C137" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3">
+      <c r="A138" t="s">
+        <v>407</v>
+      </c>
+      <c r="B138" t="s">
+        <v>408</v>
+      </c>
+      <c r="C138" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3">
+      <c r="A139" t="s">
+        <v>411</v>
+      </c>
+      <c r="B139" t="s">
+        <v>412</v>
+      </c>
+      <c r="C139" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3">
+      <c r="A140" t="s">
+        <v>413</v>
+      </c>
+      <c r="B140" t="s">
+        <v>414</v>
+      </c>
+      <c r="C140" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3">
+      <c r="A141" t="s">
+        <v>416</v>
+      </c>
+      <c r="B141" t="s">
+        <v>417</v>
+      </c>
+      <c r="C141" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3">
+      <c r="A142" t="s">
+        <v>419</v>
+      </c>
+      <c r="B142" t="s">
+        <v>420</v>
+      </c>
+      <c r="C142" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3">
+      <c r="A143" t="s">
+        <v>422</v>
+      </c>
+      <c r="B143" t="s">
+        <v>423</v>
+      </c>
+      <c r="C143" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3">
+      <c r="A144" t="s">
+        <v>425</v>
+      </c>
+      <c r="B144" t="s">
+        <v>426</v>
+      </c>
+      <c r="C144" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" t="s">
+        <v>428</v>
+      </c>
+      <c r="B145" t="s">
+        <v>429</v>
+      </c>
+      <c r="C145" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" t="s">
+        <v>431</v>
+      </c>
+      <c r="B146" t="s">
+        <v>432</v>
+      </c>
+      <c r="C146" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" t="s">
+        <v>435</v>
+      </c>
+      <c r="B147" t="s">
+        <v>436</v>
+      </c>
+      <c r="C147" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3">
+      <c r="A148" t="s">
+        <v>438</v>
+      </c>
+      <c r="B148" t="s">
+        <v>439</v>
+      </c>
+      <c r="C148" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3">
+      <c r="A149" t="s">
+        <v>441</v>
+      </c>
+      <c r="B149" t="s">
+        <v>442</v>
+      </c>
+      <c r="C149" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3">
+      <c r="A150" t="s">
+        <v>443</v>
+      </c>
+      <c r="B150" t="s">
+        <v>444</v>
+      </c>
+      <c r="C150" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3">
+      <c r="A151" t="s">
+        <v>446</v>
+      </c>
+      <c r="B151" t="s">
+        <v>447</v>
+      </c>
+      <c r="C151" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3">
+      <c r="A152" t="s">
+        <v>449</v>
+      </c>
+      <c r="B152" t="s">
+        <v>450</v>
+      </c>
+      <c r="C152" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3">
+      <c r="A153" t="s">
+        <v>452</v>
+      </c>
+      <c r="B153" t="s">
+        <v>453</v>
+      </c>
+      <c r="C153" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3">
+      <c r="A154" t="s">
+        <v>455</v>
+      </c>
+      <c r="B154" t="s">
+        <v>456</v>
+      </c>
+      <c r="C154" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3">
+      <c r="A155" t="s">
+        <v>458</v>
+      </c>
+      <c r="B155" t="s">
+        <v>459</v>
+      </c>
+      <c r="C155" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3">
+      <c r="A156" t="s">
+        <v>461</v>
+      </c>
+      <c r="B156" t="s">
+        <v>462</v>
+      </c>
+      <c r="C156" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3">
+      <c r="A157" t="s">
+        <v>464</v>
+      </c>
+      <c r="B157" t="s">
+        <v>465</v>
+      </c>
+      <c r="C157" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3">
+      <c r="A158" t="s">
+        <v>467</v>
+      </c>
+      <c r="B158" t="s">
+        <v>468</v>
+      </c>
+      <c r="C158" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3">
+      <c r="A159" t="s">
+        <v>470</v>
+      </c>
+      <c r="B159" t="s">
+        <v>471</v>
+      </c>
+      <c r="C159" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3">
+      <c r="A160" t="s">
+        <v>473</v>
+      </c>
+      <c r="B160" t="s">
+        <v>474</v>
+      </c>
+      <c r="C160" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3">
+      <c r="A161" t="s">
+        <v>476</v>
+      </c>
+      <c r="B161" t="s">
+        <v>477</v>
+      </c>
+      <c r="C161" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3">
+      <c r="A162" t="s">
+        <v>479</v>
+      </c>
+      <c r="B162" t="s">
+        <v>480</v>
+      </c>
+      <c r="C162" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3">
+      <c r="A163" t="s">
+        <v>482</v>
+      </c>
+      <c r="B163" t="s">
+        <v>483</v>
+      </c>
+      <c r="C163" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3">
+      <c r="A164" t="s">
+        <v>485</v>
+      </c>
+      <c r="B164" t="s">
+        <v>486</v>
+      </c>
+      <c r="C164" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3">
+      <c r="A165" t="s">
+        <v>488</v>
+      </c>
+      <c r="B165" t="s">
+        <v>489</v>
+      </c>
+      <c r="C165" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3">
+      <c r="A166" t="s">
+        <v>491</v>
+      </c>
+      <c r="B166" t="s">
+        <v>492</v>
+      </c>
+      <c r="C166" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3">
+      <c r="A167" t="s">
+        <v>495</v>
+      </c>
+      <c r="B167" t="s">
+        <v>496</v>
+      </c>
+      <c r="C167" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3">
+      <c r="A168" t="s">
+        <v>498</v>
+      </c>
+      <c r="B168" t="s">
+        <v>499</v>
+      </c>
+      <c r="C168" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3">
+      <c r="A169" t="s">
+        <v>501</v>
+      </c>
+      <c r="B169" t="s">
+        <v>502</v>
+      </c>
+      <c r="C169" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new gnd2tgn entries
</commit_message>
<xml_diff>
--- a/app/Resources/data/gnd2tgn.xlsx
+++ b/app/Resources/data/gnd2tgn.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="523">
   <si>
     <t>place</t>
   </si>
@@ -1525,6 +1525,66 @@
   </si>
   <si>
     <t>http://d-nb.info/gnd/4224404-3</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4479392-3</t>
+  </si>
+  <si>
+    <t>Hliník nad Hronom</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/8698315</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/8698316</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4596010-0</t>
+  </si>
+  <si>
+    <t>Vrbové</t>
+  </si>
+  <si>
+    <t>Schöneberg (Berlin)</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4106612-1</t>
+  </si>
+  <si>
+    <t>Staunton, Va.</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4463513-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7014538</t>
+  </si>
+  <si>
+    <t>Washington, DC</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7013962</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4064682-8</t>
+  </si>
+  <si>
+    <t>Posen</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4046868-9</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/7007756</t>
+  </si>
+  <si>
+    <t>Coswig</t>
+  </si>
+  <si>
+    <t>http://d-nb.info/gnd/4292634-8</t>
+  </si>
+  <si>
+    <t>http://vocab.getty.edu/tgn/1036556</t>
   </si>
 </sst>
 </file>
@@ -1859,16 +1919,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F169"/>
+  <dimension ref="A1:F176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
-      <selection activeCell="A169" sqref="A169:B169"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.3"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="16.875" customWidth="1"/>
     <col min="5" max="5" width="28.125" customWidth="1"/>
     <col min="6" max="6" width="37.75" customWidth="1"/>
@@ -3407,332 +3467,409 @@
     </row>
     <row r="140" spans="1:3">
       <c r="A140" t="s">
-        <v>413</v>
+        <v>509</v>
       </c>
       <c r="B140" t="s">
-        <v>414</v>
+        <v>510</v>
       </c>
       <c r="C140" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="141" spans="1:3">
       <c r="A141" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B141" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C141" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="142" spans="1:3">
       <c r="A142" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B142" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C142" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="143" spans="1:3">
       <c r="A143" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="B143" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C143" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="144" spans="1:3">
       <c r="A144" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="B144" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C144" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="145" spans="1:3">
       <c r="A145" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="B145" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C145" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="146" spans="1:3">
       <c r="A146" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="B146" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C146" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="147" spans="1:3">
       <c r="A147" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="B147" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C147" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
     </row>
     <row r="148" spans="1:3">
       <c r="A148" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B148" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C148" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="149" spans="1:3">
       <c r="A149" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B149" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C149" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="150" spans="1:3">
       <c r="A150" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B150" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C150" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="151" spans="1:3">
       <c r="A151" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B151" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C151" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
     </row>
     <row r="152" spans="1:3">
       <c r="A152" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="B152" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C152" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="153" spans="1:3">
       <c r="A153" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B153" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C153" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="154" spans="1:3">
       <c r="A154" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="B154" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C154" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="155" spans="1:3">
       <c r="A155" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="B155" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C155" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="156" spans="1:3">
       <c r="A156" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="B156" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C156" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="157" spans="1:3">
       <c r="A157" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="B157" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C157" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="158" spans="1:3">
       <c r="A158" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="B158" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C158" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="159" spans="1:3">
       <c r="A159" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B159" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C159" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="160" spans="1:3">
       <c r="A160" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="B160" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C160" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
     </row>
     <row r="161" spans="1:3">
       <c r="A161" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="B161" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C161" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
     </row>
     <row r="162" spans="1:3">
       <c r="A162" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="B162" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C162" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="163" spans="1:3">
       <c r="A163" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="B163" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="C163" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="164" spans="1:3">
       <c r="A164" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="B164" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C164" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
     </row>
     <row r="165" spans="1:3">
       <c r="A165" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="B165" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="C165" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="166" spans="1:3">
       <c r="A166" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B166" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C166" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="167" spans="1:3">
       <c r="A167" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="B167" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C167" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="168" spans="1:3">
       <c r="A168" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B168" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C168" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
     </row>
     <row r="169" spans="1:3">
       <c r="A169" t="s">
+        <v>498</v>
+      </c>
+      <c r="B169" t="s">
+        <v>499</v>
+      </c>
+      <c r="C169" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3">
+      <c r="A170" t="s">
         <v>501</v>
       </c>
-      <c r="B169" t="s">
+      <c r="B170" t="s">
         <v>502</v>
       </c>
-      <c r="C169" t="s">
+      <c r="C170" t="s">
         <v>500</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3">
+      <c r="A171" t="s">
+        <v>504</v>
+      </c>
+      <c r="B171" t="s">
+        <v>503</v>
+      </c>
+      <c r="C171" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3">
+      <c r="A172" t="s">
+        <v>508</v>
+      </c>
+      <c r="B172" t="s">
+        <v>507</v>
+      </c>
+      <c r="C172" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3">
+      <c r="A173" t="s">
+        <v>511</v>
+      </c>
+      <c r="B173" t="s">
+        <v>512</v>
+      </c>
+      <c r="C173" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3">
+      <c r="A174" t="s">
+        <v>514</v>
+      </c>
+      <c r="B174" t="s">
+        <v>516</v>
+      </c>
+      <c r="C174" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3">
+      <c r="A175" t="s">
+        <v>517</v>
+      </c>
+      <c r="B175" t="s">
+        <v>518</v>
+      </c>
+      <c r="C175" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3">
+      <c r="A176" t="s">
+        <v>520</v>
+      </c>
+      <c r="B176" t="s">
+        <v>521</v>
+      </c>
+      <c r="C176" t="s">
+        <v>522</v>
       </c>
     </row>
   </sheetData>

</xml_diff>